<commit_message>
Subindo Versão quase final do projeto pt 2
</commit_message>
<xml_diff>
--- a/Projeto Python/Planilhateste.xlsx
+++ b/Projeto Python/Planilhateste.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="54">
   <si>
     <t xml:space="preserve">cpf/cnpj</t>
   </si>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">COL NUM: 9</t>
   </si>
   <si>
-    <t xml:space="preserve">+5511984776938</t>
+    <t xml:space="preserve">+5511961611974</t>
   </si>
   <si>
     <t xml:space="preserve">+55 11961611974</t>
@@ -76,15 +76,9 @@
     <t xml:space="preserve">ACAETANO@GLOBO.COM   </t>
   </si>
   <si>
-    <t xml:space="preserve">+5511983358584</t>
-  </si>
-  <si>
     <t xml:space="preserve">PROCDAISYROSSINI@UOL.COM.BR   </t>
   </si>
   <si>
-    <t xml:space="preserve">+5511961611974</t>
-  </si>
-  <si>
     <t xml:space="preserve">ADCFERREI@UOL.COM.BR   </t>
   </si>
   <si>
@@ -101,9 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve">EDILSONMO@POLICIAMILITAR.SP.GOV.BR   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">+55 11965433747</t>
   </si>
   <si>
     <t xml:space="preserve">MARALICE.HUERTA@GMAIL.COM   </t>
@@ -360,7 +351,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -516,25 +507,25 @@
         <v>6</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="6"/>
@@ -546,7 +537,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>16</v>
@@ -564,7 +555,7 @@
         <v>16</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="6"/>
@@ -594,7 +585,7 @@
         <v>16</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="6"/>
@@ -606,7 +597,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>16</v>
@@ -624,7 +615,7 @@
         <v>16</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
@@ -635,7 +626,9 @@
       <c r="B10" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
@@ -652,7 +645,7 @@
         <v>16</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
@@ -682,7 +675,7 @@
         <v>16</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
@@ -694,7 +687,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>16</v>
@@ -712,7 +705,7 @@
         <v>16</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="6"/>
@@ -724,7 +717,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>16</v>
@@ -742,7 +735,7 @@
         <v>16</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="6"/>
@@ -772,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
@@ -784,7 +777,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>16</v>
@@ -802,7 +795,7 @@
         <v>16</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
@@ -814,7 +807,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>16</v>
@@ -832,7 +825,7 @@
         <v>16</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
@@ -862,7 +855,7 @@
         <v>16</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
@@ -874,7 +867,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>16</v>
@@ -892,7 +885,7 @@
         <v>16</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="6"/>
@@ -904,7 +897,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>16</v>
@@ -922,7 +915,7 @@
         <v>16</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="6"/>
@@ -952,7 +945,7 @@
         <v>16</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="6"/>
@@ -964,7 +957,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>16</v>
@@ -982,7 +975,7 @@
         <v>16</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="6"/>
@@ -994,7 +987,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>16</v>
@@ -1012,7 +1005,7 @@
         <v>16</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="6"/>
@@ -1042,7 +1035,7 @@
         <v>16</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="6"/>
@@ -1054,7 +1047,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>16</v>
@@ -1072,7 +1065,7 @@
         <v>16</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="6"/>
@@ -1084,7 +1077,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>16</v>
@@ -1102,7 +1095,7 @@
         <v>16</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="6"/>
@@ -1132,7 +1125,7 @@
         <v>16</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="6"/>
@@ -1144,7 +1137,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>16</v>
@@ -1162,7 +1155,7 @@
         <v>16</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="6"/>
@@ -1174,7 +1167,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>16</v>
@@ -1192,7 +1185,7 @@
         <v>16</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="6"/>
@@ -1222,7 +1215,7 @@
         <v>16</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="6"/>
@@ -1234,7 +1227,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>16</v>
@@ -1252,7 +1245,7 @@
         <v>16</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="6"/>
@@ -1264,7 +1257,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>16</v>
@@ -1282,7 +1275,7 @@
         <v>16</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="6"/>
@@ -1312,7 +1305,7 @@
         <v>16</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="6"/>
@@ -1324,7 +1317,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>16</v>
@@ -1342,7 +1335,7 @@
         <v>16</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="6"/>
@@ -1354,7 +1347,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>16</v>
@@ -1372,7 +1365,7 @@
         <v>16</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="6"/>
@@ -1402,7 +1395,7 @@
         <v>16</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="6"/>
@@ -1414,7 +1407,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>16</v>
@@ -1432,7 +1425,7 @@
         <v>16</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="6"/>
@@ -1444,7 +1437,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>16</v>
@@ -1462,7 +1455,7 @@
         <v>16</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="6"/>
@@ -1492,7 +1485,7 @@
         <v>16</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="6"/>
@@ -1504,7 +1497,7 @@
         <v>39</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>16</v>
@@ -1522,7 +1515,7 @@
         <v>16</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J39" s="5"/>
       <c r="K39" s="6"/>
@@ -1534,7 +1527,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>16</v>
@@ -1552,7 +1545,7 @@
         <v>16</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="6"/>
@@ -1582,7 +1575,7 @@
         <v>16</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J41" s="5"/>
       <c r="K41" s="6"/>
@@ -1594,7 +1587,7 @@
         <v>42</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>16</v>
@@ -1612,7 +1605,7 @@
         <v>16</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J42" s="5"/>
       <c r="K42" s="6"/>
@@ -1624,7 +1617,7 @@
         <v>43</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>16</v>
@@ -1642,7 +1635,7 @@
         <v>16</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J43" s="5"/>
       <c r="K43" s="6"/>
@@ -1672,7 +1665,7 @@
         <v>16</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Subindo versão finalizado do projeto
</commit_message>
<xml_diff>
--- a/Projeto Python/Planilhateste.xlsx
+++ b/Projeto Python/Planilhateste.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="54">
   <si>
     <t xml:space="preserve">cpf/cnpj</t>
   </si>
@@ -351,7 +351,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5:C44"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -368,7 +368,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -398,7 +398,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -414,7 +414,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -444,7 +444,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>15</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>15</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>15</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>15</v>
@@ -594,11 +594,9 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>15</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
         <v>16</v>
       </c>
@@ -624,7 +622,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>15</v>
@@ -654,7 +652,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>15</v>
@@ -684,7 +682,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>15</v>
@@ -714,7 +712,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>15</v>
@@ -744,7 +742,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>15</v>
@@ -774,7 +772,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>15</v>
@@ -804,7 +802,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>15</v>
@@ -834,7 +832,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>15</v>
@@ -864,7 +862,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>15</v>
@@ -894,7 +892,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>15</v>
@@ -924,7 +922,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>15</v>
@@ -954,7 +952,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>15</v>
@@ -984,7 +982,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>15</v>
@@ -1014,7 +1012,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>15</v>
@@ -1044,7 +1042,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>15</v>
@@ -1074,7 +1072,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>15</v>
@@ -1104,7 +1102,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>15</v>
@@ -1134,7 +1132,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>15</v>
@@ -1164,7 +1162,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>15</v>
@@ -1194,7 +1192,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>15</v>
@@ -1224,7 +1222,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="2" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>15</v>
@@ -1254,7 +1252,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>15</v>
@@ -1284,7 +1282,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>15</v>
@@ -1314,7 +1312,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>15</v>
@@ -1344,7 +1342,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="2" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>15</v>
@@ -1374,7 +1372,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="2" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>15</v>
@@ -1404,7 +1402,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>15</v>
@@ -1434,7 +1432,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="2" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>15</v>
@@ -1464,7 +1462,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="2" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>15</v>
@@ -1494,7 +1492,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="2" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>15</v>
@@ -1524,7 +1522,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="2" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>15</v>
@@ -1554,7 +1552,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="2" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>15</v>
@@ -1584,7 +1582,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="2" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>15</v>
@@ -1614,7 +1612,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="2" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>15</v>
@@ -1644,7 +1642,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="2" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>15</v>

</xml_diff>